<commit_message>
scanns and notes from photobomb
</commit_message>
<xml_diff>
--- a/machines/photobomb/photobombMeth.xlsx
+++ b/machines/photobomb/photobombMeth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Recon" sheetId="1" state="visible" r:id="rId3"/>
@@ -32,39 +32,291 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t xml:space="preserve">Don’t Forget</t>
   </si>
   <si>
+    <t xml:space="preserve">CREDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web</t>
+  </si>
+  <si>
     <t xml:space="preserve">sudo -l</t>
   </si>
   <si>
+    <t xml:space="preserve">pH0t0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b0Mb!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">gtfo bins</t>
   </si>
   <si>
     <t xml:space="preserve">searchsploit</t>
   </si>
   <si>
+    <t xml:space="preserve">Burp</t>
+  </si>
+  <si>
     <t xml:space="preserve">sudo nmap $TIP -A -p-  -oA $TIP-A-p-</t>
   </si>
   <si>
+    <t xml:space="preserve">Host is up (0.066s latency).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not shown: 65533 closed tcp ports (reset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORT   STATE SERVICE VERSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/tcp open  ssh     OpenSSH 8.2p1 Ubuntu 4ubuntu0.5 (Ubuntu Linux; protocol 2.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| ssh-hostkey: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">|   3072 e2:24:73:bb:fb:df:5c:b5:20:b6:68:76:74:8a:b5:8d (RSA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|   256 04:e3:ac:6e:18:4e:1b:7e:ff:ac:4f:e3:9d:d2:1b:ae (ECDSA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_  256 20:e0:5d:8c:ba:71:f0:8c:3a:18:19:f2:40:11:d2:9e (ED25519)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80/tcp open  http    nginx 1.18.0 (Ubuntu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_http-title: Did not follow redirect to http://photobomb.htb/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_http-server-header: nginx/1.18.0 (Ubuntu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No exact OS matches for host (If you know what OS is running on it, see https://nmap.org/submit/ ).</t>
+  </si>
+  <si>
     <t xml:space="preserve">sudo nmap -p 25 --script smtp-enum-users $TIP</t>
   </si>
   <si>
     <t xml:space="preserve">msf6 auxiliary(scanner/smtp/smtp_enum) </t>
   </si>
   <si>
-    <t xml:space="preserve">└─$ curl -I https://10.10.10.7 -k</t>
+    <t xml:space="preserve">curl -I $TURL -k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP/1.1 200 OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server: nginx/1.18.0 (Ubuntu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: Wed, 25 Sep 2024 17:10:08 GMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content-Type: text/html;charset=utf-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content-Length: 843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connection: keep-alive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Xss-Protection: 1; mode=block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Content-Type-Options: nosniff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Frame-Options: SAMEORIGIN</t>
   </si>
   <si>
     <t xml:space="preserve">sudo gobuster dir -u $TURL -w /usr/share/dirbuster/wordlists/directory-list-2.3-medium.txt</t>
   </si>
   <si>
+    <t xml:space="preserve">[+] Url:                     http://photobomb.htb/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] Method:                  GET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] Threads:                 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] Wordlist:                /usr/share/dirbuster/wordlists/directory-list-2.3-medium.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] Negative Status codes:   404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] User Agent:              gobuster/3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[+] Timeout:                 10s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting gobuster in directory enumeration mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer              (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printers             (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printerfriendly      (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_friendly     (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_icon         (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer-icon         (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer-friendly     (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printerFriendly      (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printersupplies      (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer1             (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer2             (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printericon          (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_2867         (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_securit      (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_drivers      (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_2            (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer_list         (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printerdrivers       (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/printer-ink          (Status: 401) [Size: 188]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress: 220560 / 220561 (100.00%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished</t>
+  </si>
+  <si>
     <t xml:space="preserve">ffuf -u http://10.10.10.242/FUZZ -w /usr/share/wordlists/dirb/common.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">sudo nikto -h http://10.10.10.242/ -o niktoResult.txt -Format txt</t>
+    <t xml:space="preserve">sudo nikto -h $TURL -o niktoResult.txt -Format txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nikto v2.5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">---------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Target IP:          10.10.11.182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Target Hostname:    photobomb.htb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Target Port:        80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Start Time:         2024-09-25 12:23:10 (GMT-4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Server: nginx/1.18.0 (Ubuntu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /QS20am5w.nn: Uncommon header 'x-cascade' found, with contents: pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /QS20am5w.exe|dir: The X-Content-Type-Options header is not set. This could allow the user agent to render the content of the site in a different fashion to the MIME type. See: https://www.netsparker.com/web-vulnerability-scanner/vulnerabilities/missing-content-type-header/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ No CGI Directories found (use '-C all' to force check all possible dirs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ nginx/1.18.0 appears to be outdated (current is at least 1.20.1).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ ///etc/hosts: The server install allows reading of any system file by adding an extra '/' to the URL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wp-content/themes/twentyeleven/images/headers/server.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wordpress/wp-content/themes/twentyeleven/images/headers/server.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wp-includes/Requests/Utility/content-post.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wordpress/wp-includes/Requests/Utility/content-post.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wp-includes/js/tinymce/themes/modern/Meuhy.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /wordpress/wp-includes/js/tinymce/themes/modern/Meuhy.php?filesrc=/etc/hosts: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /assets/mobirise/css/meta.php?filesrc=: A PHP backdoor file manager was found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /login.cgi?cli=aa%20aa%27cat%20/etc/hosts: Some D-Link router remote command execution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ /shell?cat+/etc/hosts: A backdoor was identified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ 7962 requests: 0 error(s) and 13 item(s) reported on remote host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ End Time:           2024-09-25 12:32:45 (GMT-4) (575 seconds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ 1 host(s) tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nginx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu</t>
   </si>
 </sst>
 </file>
@@ -154,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,7 +419,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,10 +644,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,20 +659,43 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -499,70 +806,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="260.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="260.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="7" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="10.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="7" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
+      <c r="A27" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
+      <c r="A29" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
+      <c r="A32" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3"/>
+      <c r="A41" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3"/>
+      <c r="A43" s="11"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3"/>
+      <c r="A52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3"/>
+      <c r="A53" s="11"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3"/>
+      <c r="A55" s="11"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3"/>
+      <c r="A56" s="11"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3"/>
+      <c r="A57" s="11"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3"/>
+      <c r="A58" s="11"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3"/>
+      <c r="A59" s="11"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3"/>
+      <c r="A60" s="11"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3"/>
+      <c r="A61" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -593,7 +964,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -610,7 +981,7 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -636,10 +1007,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,7 +1020,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -668,17 +1084,192 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="e">
+        <f aca="false">==============================================================</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="e">
+        <f aca="false">==============================================================</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="e">
+        <f aca="false">==============================================================</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="e">
+        <f aca="false">==============================================================</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="e">
+        <f aca="false">==============================================================</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +1298,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -726,19 +1317,150 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -778,10 +1500,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -790,10 +1512,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>

</xml_diff>